<commit_message>
Updating BCIO_Upper_Defs.xlsx - Added errors for demonstration
</commit_message>
<xml_diff>
--- a/Upper Level BCIO/inputs/BCIO_Upper_Defs.xlsx
+++ b/Upper Level BCIO/inputs/BCIO_Upper_Defs.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V65"/>
+  <dimension ref="A1:V67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,22 +466,22 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Parent</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>BFO entity</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Sub-ontology</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>Definition source</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Parent</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>BFO entity</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Sub-ontology</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -556,11 +556,7 @@
           <t>BCIO:050315</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>BCI attribute</t>
-        </is>
-      </c>
+      <c r="B2" s="2" t="inlineStr"/>
       <c r="C2" s="2" t="inlineStr">
         <is>
           <t>A process attribute whose bearer is a behaviour change intervention.</t>
@@ -571,23 +567,23 @@
           <t>An attribute of a behaviour change intervention.</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr"/>
-      <c r="F2" s="2" t="n"/>
+      <c r="E2" s="2" t="n"/>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>process attribute</t>
+        </is>
+      </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>process attribute</t>
+          <t>process</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>process</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="n"/>
       <c r="J2" s="2" t="n"/>
       <c r="K2" s="2" t="n"/>
       <c r="L2" s="2" t="n"/>
@@ -640,7 +636,11 @@
         </is>
       </c>
       <c r="E3" s="2" t="n"/>
-      <c r="F3" s="2" t="n"/>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>information content entity</t>
+        </is>
+      </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
           <t>information content entity</t>
@@ -648,14 +648,10 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>information content entity</t>
-        </is>
-      </c>
-      <c r="I3" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I3" s="2" t="n"/>
       <c r="J3" s="2" t="n"/>
       <c r="K3" s="2" t="n"/>
       <c r="L3" s="2" t="n"/>
@@ -700,22 +696,22 @@
       </c>
       <c r="D4" s="2" t="n"/>
       <c r="E4" s="2" t="n"/>
-      <c r="F4" s="2" t="n"/>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>intervention</t>
+        </is>
+      </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>intervention</t>
+          <t>process</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
         <is>
-          <t>process</t>
-        </is>
-      </c>
-      <c r="I4" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I4" s="2" t="n"/>
       <c r="J4" s="2" t="inlineStr">
         <is>
           <t>behaviour change intervention content; participant engagement with behaviour change intervention; behaviour change intervention mechanism of action; behaviour change intervention outcome behaviour</t>
@@ -776,22 +772,22 @@
       </c>
       <c r="D5" s="2" t="n"/>
       <c r="E5" s="2" t="n"/>
-      <c r="F5" s="2" t="n"/>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>behaviour change intervention evaluation study</t>
+        </is>
+      </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>behaviour change intervention evaluation study</t>
+          <t>process</t>
         </is>
       </c>
       <c r="H5" s="2" t="inlineStr">
         <is>
-          <t>process</t>
-        </is>
-      </c>
-      <c r="I5" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I5" s="2" t="n"/>
       <c r="J5" s="2" t="n"/>
       <c r="K5" s="2" t="n"/>
       <c r="L5" s="2" t="n"/>
@@ -844,22 +840,22 @@
       </c>
       <c r="D6" s="2" t="n"/>
       <c r="E6" s="2" t="n"/>
-      <c r="F6" s="2" t="n"/>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>intervention content</t>
+        </is>
+      </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>intervention content</t>
+          <t>process</t>
         </is>
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>process</t>
-        </is>
-      </c>
-      <c r="I6" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I6" s="2" t="n"/>
       <c r="J6" s="2" t="n"/>
       <c r="K6" s="2" t="n"/>
       <c r="L6" s="2" t="n"/>
@@ -912,7 +908,11 @@
       </c>
       <c r="D7" s="2" t="n"/>
       <c r="E7" s="2" t="n"/>
-      <c r="F7" s="2" t="n"/>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>object aggregate</t>
+        </is>
+      </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
           <t>object aggregate</t>
@@ -920,14 +920,10 @@
       </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>object aggregate</t>
-        </is>
-      </c>
-      <c r="I7" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I7" s="2" t="n"/>
       <c r="J7" s="2" t="n"/>
       <c r="K7" s="2" t="n"/>
       <c r="L7" s="2" t="n"/>
@@ -980,22 +976,22 @@
       </c>
       <c r="D8" s="2" t="n"/>
       <c r="E8" s="2" t="n"/>
-      <c r="F8" s="2" t="n"/>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>intervention delivery</t>
+        </is>
+      </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
-          <t>intervention delivery</t>
+          <t>process</t>
         </is>
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>process</t>
-        </is>
-      </c>
-      <c r="I8" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I8" s="2" t="n"/>
       <c r="J8" s="2" t="n"/>
       <c r="K8" s="2" t="n"/>
       <c r="L8" s="2" t="n"/>
@@ -1044,22 +1040,22 @@
       </c>
       <c r="D9" s="2" t="n"/>
       <c r="E9" s="2" t="n"/>
-      <c r="F9" s="2" t="n"/>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>BCI attribute [BCIO:0503150]</t>
+        </is>
+      </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>BCI attribute</t>
+          <t>process</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
         <is>
-          <t>process</t>
-        </is>
-      </c>
-      <c r="I9" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I9" s="2" t="n"/>
       <c r="J9" s="2" t="n"/>
       <c r="K9" s="2" t="n"/>
       <c r="L9" s="2" t="n"/>
@@ -1116,22 +1112,22 @@
       </c>
       <c r="D10" s="2" t="n"/>
       <c r="E10" s="2" t="n"/>
-      <c r="F10" s="2" t="n"/>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>behaviour change intervention evaluation finding</t>
+        </is>
+      </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
-          <t>behaviour change intervention evaluation finding</t>
+          <t>information content entity</t>
         </is>
       </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
-          <t>information content entity</t>
-        </is>
-      </c>
-      <c r="I10" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I10" s="2" t="n"/>
       <c r="J10" s="2" t="n"/>
       <c r="K10" s="2" t="n"/>
       <c r="L10" s="2" t="n"/>
@@ -1184,22 +1180,22 @@
       </c>
       <c r="D11" s="2" t="n"/>
       <c r="E11" s="2" t="n"/>
-      <c r="F11" s="2" t="n"/>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>evaluation finding</t>
+        </is>
+      </c>
       <c r="G11" s="2" t="inlineStr">
         <is>
-          <t>evaluation finding</t>
+          <t>information content entoty</t>
         </is>
       </c>
       <c r="H11" s="2" t="inlineStr">
         <is>
-          <t>information content entoty</t>
-        </is>
-      </c>
-      <c r="I11" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I11" s="2" t="n"/>
       <c r="J11" s="2" t="n"/>
       <c r="K11" s="2" t="n"/>
       <c r="L11" s="2" t="n"/>
@@ -1248,22 +1244,22 @@
       </c>
       <c r="D12" s="2" t="n"/>
       <c r="E12" s="2" t="n"/>
-      <c r="F12" s="2" t="n"/>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>report</t>
+        </is>
+      </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
-          <t>report</t>
+          <t>generally dependent continuant</t>
         </is>
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>generally dependent continuant</t>
-        </is>
-      </c>
-      <c r="I12" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I12" s="2" t="n"/>
       <c r="J12" s="2" t="n"/>
       <c r="K12" s="2" t="n"/>
       <c r="L12" s="2" t="n"/>
@@ -1299,68 +1295,68 @@
       <c r="V12" s="2" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="inlineStr">
+      <c r="A13" s="3" t="inlineStr">
         <is>
           <t>BCIO:018000</t>
         </is>
       </c>
-      <c r="B13" s="2" t="inlineStr">
+      <c r="B13" s="3" t="inlineStr">
         <is>
           <t>behaviour change intervention evaluation study</t>
         </is>
       </c>
-      <c r="C13" s="2" t="inlineStr">
+      <c r="C13" s="3" t="inlineStr">
         <is>
           <t>An intervention evaluation study of a BCI scenario.</t>
         </is>
       </c>
-      <c r="D13" s="2" t="n"/>
-      <c r="E13" s="2" t="n"/>
-      <c r="F13" s="2" t="n"/>
-      <c r="G13" s="2" t="inlineStr">
+      <c r="D13" s="3" t="n"/>
+      <c r="E13" s="3" t="n"/>
+      <c r="F13" s="3" t="inlineStr">
         <is>
           <t>intervention evaluation study</t>
         </is>
       </c>
-      <c r="H13" s="2" t="inlineStr">
+      <c r="G13" s="3" t="inlineStr">
         <is>
           <t>process</t>
         </is>
       </c>
-      <c r="I13" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
-      <c r="J13" s="2" t="n"/>
-      <c r="K13" s="2" t="n"/>
-      <c r="L13" s="2" t="n"/>
-      <c r="M13" s="2" t="inlineStr">
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="n"/>
+      <c r="J13" s="3" t="n"/>
+      <c r="K13" s="3" t="n"/>
+      <c r="L13" s="3" t="n"/>
+      <c r="M13" s="3" t="inlineStr">
         <is>
           <t>BCI evaluation study</t>
         </is>
       </c>
-      <c r="N13" s="2" t="n"/>
-      <c r="O13" s="2" t="n"/>
-      <c r="P13" s="2" t="n"/>
-      <c r="Q13" s="2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="R13" s="2" t="n"/>
-      <c r="S13" s="2" t="inlineStr">
+      <c r="N13" s="3" t="n"/>
+      <c r="O13" s="3" t="n"/>
+      <c r="P13" s="3" t="n"/>
+      <c r="Q13" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R13" s="3" t="n"/>
+      <c r="S13" s="3" t="inlineStr">
         <is>
           <t>JH; RW</t>
         </is>
       </c>
-      <c r="T13" s="2" t="inlineStr">
-        <is>
-          <t>Published</t>
-        </is>
-      </c>
-      <c r="U13" s="2" t="n"/>
-      <c r="V13" s="2" t="n"/>
+      <c r="T13" s="3" t="inlineStr">
+        <is>
+          <t>Obsolete</t>
+        </is>
+      </c>
+      <c r="U13" s="3" t="n"/>
+      <c r="V13" s="3" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
@@ -1380,22 +1376,22 @@
       </c>
       <c r="D14" s="2" t="n"/>
       <c r="E14" s="2" t="n"/>
-      <c r="F14" s="2" t="n"/>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>plan</t>
+        </is>
+      </c>
       <c r="G14" s="2" t="inlineStr">
         <is>
-          <t>plan</t>
+          <t>information content entity</t>
         </is>
       </c>
       <c r="H14" s="2" t="inlineStr">
         <is>
-          <t>information content entity</t>
-        </is>
-      </c>
-      <c r="I14" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I14" s="2" t="n"/>
       <c r="J14" s="2" t="n"/>
       <c r="K14" s="2" t="n"/>
       <c r="L14" s="2" t="n"/>
@@ -1444,7 +1440,11 @@
       </c>
       <c r="D15" s="2" t="n"/>
       <c r="E15" s="2" t="n"/>
-      <c r="F15" s="2" t="n"/>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>information content entity</t>
+        </is>
+      </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
           <t>information content entity</t>
@@ -1452,14 +1452,10 @@
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>information content entity</t>
-        </is>
-      </c>
-      <c r="I15" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I15" s="2" t="n"/>
       <c r="J15" s="2" t="n"/>
       <c r="K15" s="2" t="n"/>
       <c r="L15" s="2" t="n"/>
@@ -1508,7 +1504,11 @@
       </c>
       <c r="D16" s="2" t="n"/>
       <c r="E16" s="2" t="n"/>
-      <c r="F16" s="2" t="n"/>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>process</t>
+        </is>
+      </c>
       <c r="G16" s="2" t="inlineStr">
         <is>
           <t>process</t>
@@ -1516,14 +1516,10 @@
       </c>
       <c r="H16" s="2" t="inlineStr">
         <is>
-          <t>process</t>
-        </is>
-      </c>
-      <c r="I16" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I16" s="2" t="n"/>
       <c r="J16" s="2" t="n"/>
       <c r="K16" s="2" t="n"/>
       <c r="L16" s="2" t="n"/>
@@ -1572,22 +1568,22 @@
       </c>
       <c r="D17" s="2" t="n"/>
       <c r="E17" s="2" t="n"/>
-      <c r="F17" s="2" t="n"/>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>BCI attribute</t>
+        </is>
+      </c>
       <c r="G17" s="2" t="inlineStr">
         <is>
-          <t>BCI attribute</t>
+          <t>process</t>
         </is>
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>process</t>
-        </is>
-      </c>
-      <c r="I17" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I17" s="2" t="n"/>
       <c r="J17" s="2" t="n"/>
       <c r="K17" s="2" t="n"/>
       <c r="L17" s="2" t="n"/>
@@ -1636,18 +1632,18 @@
       </c>
       <c r="D18" s="2" t="n"/>
       <c r="E18" s="2" t="n"/>
-      <c r="F18" s="2" t="n"/>
-      <c r="G18" s="2" t="inlineStr">
+      <c r="F18" s="2" t="inlineStr">
         <is>
           <t>human behaviour</t>
         </is>
       </c>
-      <c r="H18" s="2" t="n"/>
-      <c r="I18" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G18" s="2" t="n"/>
+      <c r="H18" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I18" s="2" t="n"/>
       <c r="J18" s="2" t="n"/>
       <c r="K18" s="2" t="n"/>
       <c r="L18" s="2" t="n"/>
@@ -1692,22 +1688,22 @@
       </c>
       <c r="D19" s="2" t="n"/>
       <c r="E19" s="2" t="n"/>
-      <c r="F19" s="2" t="n"/>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>behaviour change intervention evaluation finding</t>
+        </is>
+      </c>
       <c r="G19" s="2" t="inlineStr">
         <is>
-          <t>behaviour change intervention evaluation finding</t>
+          <t>information content entoty</t>
         </is>
       </c>
       <c r="H19" s="2" t="inlineStr">
         <is>
-          <t>information content entoty</t>
-        </is>
-      </c>
-      <c r="I19" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I19" s="2" t="n"/>
       <c r="J19" s="2" t="n"/>
       <c r="K19" s="2" t="n"/>
       <c r="L19" s="2" t="n"/>
@@ -1760,18 +1756,18 @@
       </c>
       <c r="D20" s="2" t="n"/>
       <c r="E20" s="2" t="n"/>
-      <c r="F20" s="2" t="n"/>
-      <c r="G20" s="2" t="inlineStr">
+      <c r="F20" s="2" t="inlineStr">
         <is>
           <t>environmental system</t>
         </is>
       </c>
-      <c r="H20" s="2" t="n"/>
-      <c r="I20" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G20" s="2" t="n"/>
+      <c r="H20" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I20" s="2" t="n"/>
       <c r="J20" s="2" t="n"/>
       <c r="K20" s="2" t="n"/>
       <c r="L20" s="2" t="n"/>
@@ -1820,18 +1816,18 @@
       </c>
       <c r="D21" s="2" t="n"/>
       <c r="E21" s="2" t="n"/>
-      <c r="F21" s="2" t="n"/>
-      <c r="G21" s="2" t="inlineStr">
+      <c r="F21" s="2" t="inlineStr">
         <is>
           <t>intervention population</t>
         </is>
       </c>
-      <c r="H21" s="2" t="n"/>
-      <c r="I21" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G21" s="2" t="n"/>
+      <c r="H21" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I21" s="2" t="n"/>
       <c r="J21" s="2" t="n"/>
       <c r="K21" s="2" t="n"/>
       <c r="L21" s="2" t="n"/>
@@ -1880,18 +1876,18 @@
       </c>
       <c r="D22" s="2" t="n"/>
       <c r="E22" s="2" t="n"/>
-      <c r="F22" s="2" t="n"/>
-      <c r="G22" s="2" t="inlineStr">
+      <c r="F22" s="2" t="inlineStr">
         <is>
           <t>planned process</t>
         </is>
       </c>
-      <c r="H22" s="2" t="n"/>
-      <c r="I22" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G22" s="2" t="n"/>
+      <c r="H22" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I22" s="2" t="n"/>
       <c r="J22" s="2" t="n"/>
       <c r="K22" s="2" t="n"/>
       <c r="L22" s="2" t="n"/>
@@ -1940,18 +1936,18 @@
       </c>
       <c r="D23" s="2" t="n"/>
       <c r="E23" s="2" t="n"/>
-      <c r="F23" s="2" t="n"/>
-      <c r="G23" s="2" t="inlineStr">
+      <c r="F23" s="2" t="inlineStr">
         <is>
           <t>plan</t>
         </is>
       </c>
-      <c r="H23" s="2" t="n"/>
-      <c r="I23" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G23" s="2" t="n"/>
+      <c r="H23" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I23" s="2" t="n"/>
       <c r="J23" s="2" t="n"/>
       <c r="K23" s="2" t="n"/>
       <c r="L23" s="2" t="n"/>
@@ -2000,18 +1996,18 @@
       </c>
       <c r="D24" s="2" t="n"/>
       <c r="E24" s="2" t="n"/>
-      <c r="F24" s="2" t="n"/>
-      <c r="G24" s="2" t="inlineStr">
+      <c r="F24" s="2" t="inlineStr">
         <is>
           <t>report</t>
         </is>
       </c>
-      <c r="H24" s="2" t="n"/>
-      <c r="I24" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G24" s="2" t="n"/>
+      <c r="H24" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I24" s="2" t="n"/>
       <c r="J24" s="2" t="n"/>
       <c r="K24" s="2" t="n"/>
       <c r="L24" s="2" t="n"/>
@@ -2060,18 +2056,18 @@
       </c>
       <c r="D25" s="2" t="n"/>
       <c r="E25" s="2" t="n"/>
-      <c r="F25" s="2" t="n"/>
-      <c r="G25" s="2" t="inlineStr">
+      <c r="F25" s="2" t="inlineStr">
         <is>
           <t>BCI attribute</t>
         </is>
       </c>
-      <c r="H25" s="2" t="n"/>
-      <c r="I25" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G25" s="2" t="n"/>
+      <c r="H25" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I25" s="2" t="n"/>
       <c r="J25" s="2" t="n"/>
       <c r="K25" s="2" t="n"/>
       <c r="L25" s="2" t="n"/>
@@ -2124,18 +2120,18 @@
       </c>
       <c r="D26" s="2" t="n"/>
       <c r="E26" s="2" t="n"/>
-      <c r="F26" s="2" t="n"/>
-      <c r="G26" s="2" t="inlineStr">
+      <c r="F26" s="2" t="inlineStr">
         <is>
           <t>object aggregate</t>
         </is>
       </c>
-      <c r="H26" s="2" t="n"/>
-      <c r="I26" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G26" s="2" t="n"/>
+      <c r="H26" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I26" s="2" t="n"/>
       <c r="J26" s="2" t="n"/>
       <c r="K26" s="2" t="n"/>
       <c r="L26" s="2" t="n"/>
@@ -2188,18 +2184,18 @@
       </c>
       <c r="D27" s="2" t="n"/>
       <c r="E27" s="2" t="n"/>
-      <c r="F27" s="2" t="n"/>
-      <c r="G27" s="2" t="inlineStr">
+      <c r="F27" s="2" t="inlineStr">
         <is>
           <t>human population</t>
         </is>
       </c>
-      <c r="H27" s="2" t="n"/>
-      <c r="I27" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G27" s="2" t="n"/>
+      <c r="H27" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I27" s="2" t="n"/>
       <c r="J27" s="2" t="n"/>
       <c r="K27" s="2" t="n"/>
       <c r="L27" s="2" t="n"/>
@@ -2248,18 +2244,18 @@
       </c>
       <c r="D28" s="2" t="n"/>
       <c r="E28" s="2" t="n"/>
-      <c r="F28" s="2" t="n"/>
-      <c r="G28" s="2" t="inlineStr">
+      <c r="F28" s="2" t="inlineStr">
         <is>
           <t>role</t>
         </is>
       </c>
-      <c r="H28" s="2" t="n"/>
-      <c r="I28" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G28" s="2" t="n"/>
+      <c r="H28" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I28" s="2" t="n"/>
       <c r="J28" s="2" t="n"/>
       <c r="K28" s="2" t="n"/>
       <c r="L28" s="2" t="n"/>
@@ -2316,18 +2312,18 @@
           <t>A and B</t>
         </is>
       </c>
-      <c r="F29" s="2" t="n"/>
-      <c r="G29" s="2" t="inlineStr">
+      <c r="F29" s="2" t="inlineStr">
         <is>
           <t>role</t>
         </is>
       </c>
-      <c r="H29" s="2" t="n"/>
-      <c r="I29" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G29" s="2" t="n"/>
+      <c r="H29" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I29" s="2" t="n"/>
       <c r="J29" s="2" t="n"/>
       <c r="K29" s="2" t="n"/>
       <c r="L29" s="2" t="n"/>
@@ -2380,18 +2376,18 @@
       </c>
       <c r="D30" s="2" t="n"/>
       <c r="E30" s="2" t="n"/>
-      <c r="F30" s="2" t="n"/>
-      <c r="G30" s="2" t="inlineStr">
+      <c r="F30" s="2" t="inlineStr">
         <is>
           <t>research study sample</t>
         </is>
       </c>
-      <c r="H30" s="2" t="n"/>
-      <c r="I30" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G30" s="2" t="n"/>
+      <c r="H30" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I30" s="2" t="n"/>
       <c r="J30" s="2" t="n"/>
       <c r="K30" s="2" t="n"/>
       <c r="L30" s="2" t="n"/>
@@ -2440,18 +2436,18 @@
       </c>
       <c r="D31" s="2" t="n"/>
       <c r="E31" s="2" t="n"/>
-      <c r="F31" s="2" t="n"/>
-      <c r="G31" s="2" t="inlineStr">
+      <c r="F31" s="2" t="inlineStr">
         <is>
           <t>communication style</t>
         </is>
       </c>
-      <c r="H31" s="2" t="n"/>
-      <c r="I31" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G31" s="2" t="n"/>
+      <c r="H31" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I31" s="2" t="n"/>
       <c r="J31" s="2" t="n"/>
       <c r="K31" s="2" t="n"/>
       <c r="L31" s="2" t="n"/>
@@ -2508,18 +2504,18 @@
         </is>
       </c>
       <c r="E32" s="2" t="n"/>
-      <c r="F32" s="2" t="n"/>
-      <c r="G32" s="2" t="inlineStr">
+      <c r="F32" s="2" t="inlineStr">
         <is>
           <t>BCI attribute</t>
         </is>
       </c>
-      <c r="H32" s="2" t="n"/>
-      <c r="I32" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G32" s="2" t="n"/>
+      <c r="H32" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I32" s="2" t="n"/>
       <c r="J32" s="2" t="n"/>
       <c r="K32" s="2" t="n"/>
       <c r="L32" s="2" t="n"/>
@@ -2576,18 +2572,18 @@
       </c>
       <c r="D33" s="2" t="n"/>
       <c r="E33" s="2" t="n"/>
-      <c r="F33" s="2" t="n"/>
-      <c r="G33" s="2" t="inlineStr">
+      <c r="F33" s="2" t="inlineStr">
         <is>
           <t>process</t>
         </is>
       </c>
-      <c r="H33" s="2" t="n"/>
-      <c r="I33" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G33" s="2" t="n"/>
+      <c r="H33" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I33" s="2" t="n"/>
       <c r="J33" s="2" t="n"/>
       <c r="K33" s="2" t="n"/>
       <c r="L33" s="2" t="n"/>
@@ -2636,18 +2632,18 @@
       </c>
       <c r="D34" s="2" t="n"/>
       <c r="E34" s="2" t="n"/>
-      <c r="F34" s="2" t="n"/>
-      <c r="G34" s="2" t="inlineStr">
+      <c r="F34" s="2" t="inlineStr">
         <is>
           <t>behaviour change intervention temporal context</t>
         </is>
       </c>
-      <c r="H34" s="2" t="n"/>
-      <c r="I34" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G34" s="2" t="n"/>
+      <c r="H34" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I34" s="2" t="n"/>
       <c r="J34" s="2" t="n"/>
       <c r="K34" s="2" t="n"/>
       <c r="L34" s="2" t="n"/>
@@ -2696,18 +2692,18 @@
       </c>
       <c r="D35" s="2" t="n"/>
       <c r="E35" s="2" t="n"/>
-      <c r="F35" s="2" t="n"/>
-      <c r="G35" s="2" t="inlineStr">
+      <c r="F35" s="2" t="inlineStr">
         <is>
           <t>planned process</t>
         </is>
       </c>
-      <c r="H35" s="2" t="n"/>
-      <c r="I35" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G35" s="2" t="n"/>
+      <c r="H35" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I35" s="2" t="n"/>
       <c r="J35" s="2" t="n"/>
       <c r="K35" s="2" t="n"/>
       <c r="L35" s="2" t="n"/>
@@ -2756,18 +2752,18 @@
       </c>
       <c r="D36" s="2" t="n"/>
       <c r="E36" s="2" t="n"/>
-      <c r="F36" s="2" t="n"/>
-      <c r="G36" s="2" t="inlineStr">
+      <c r="F36" s="2" t="inlineStr">
         <is>
           <t>process attribute</t>
         </is>
       </c>
-      <c r="H36" s="2" t="n"/>
-      <c r="I36" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G36" s="2" t="n"/>
+      <c r="H36" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I36" s="2" t="n"/>
       <c r="J36" s="2" t="n"/>
       <c r="K36" s="2" t="n"/>
       <c r="L36" s="2" t="n"/>
@@ -2812,18 +2808,18 @@
       </c>
       <c r="D37" s="2" t="n"/>
       <c r="E37" s="2" t="n"/>
-      <c r="F37" s="2" t="n"/>
-      <c r="G37" s="2" t="inlineStr">
+      <c r="F37" s="2" t="inlineStr">
         <is>
           <t>communication process attribute</t>
         </is>
       </c>
-      <c r="H37" s="2" t="n"/>
-      <c r="I37" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G37" s="2" t="n"/>
+      <c r="H37" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I37" s="2" t="n"/>
       <c r="J37" s="2" t="n"/>
       <c r="K37" s="2" t="n"/>
       <c r="L37" s="2" t="n"/>
@@ -2851,151 +2847,133 @@
       <c r="V37" s="2" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="inlineStr">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>BFO:0000002</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>continuant2</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>entity</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr"/>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr"/>
+      <c r="Q38" t="n">
+        <v>0</v>
+      </c>
+      <c r="R38" t="inlineStr"/>
+      <c r="S38" t="inlineStr"/>
+      <c r="T38" t="inlineStr">
+        <is>
+          <t>External</t>
+        </is>
+      </c>
+      <c r="U38" t="inlineStr"/>
+      <c r="V38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="inlineStr">
         <is>
           <t>BCIO:035000</t>
         </is>
       </c>
-      <c r="B38" s="2" t="inlineStr">
+      <c r="B39" s="2" t="inlineStr">
         <is>
           <t>evaluation finding</t>
         </is>
       </c>
-      <c r="C38" s="2" t="inlineStr">
+      <c r="C39" s="2" t="inlineStr">
         <is>
           <t>A data item that is the output of an intervention evaluation study.</t>
         </is>
       </c>
-      <c r="D38" s="2" t="n"/>
-      <c r="E38" s="2" t="n"/>
-      <c r="F38" s="2" t="n"/>
-      <c r="G38" s="2" t="inlineStr">
+      <c r="D39" s="2" t="n"/>
+      <c r="E39" s="2" t="n"/>
+      <c r="F39" s="2" t="inlineStr">
         <is>
           <t>data item</t>
         </is>
       </c>
-      <c r="H38" s="2" t="n"/>
-      <c r="I38" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
-      <c r="J38" s="2" t="n"/>
-      <c r="K38" s="2" t="n"/>
-      <c r="L38" s="2" t="n"/>
-      <c r="M38" s="2" t="n"/>
-      <c r="N38" s="2" t="n"/>
-      <c r="O38" s="2" t="n"/>
-      <c r="P38" s="2" t="n"/>
-      <c r="Q38" s="2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="R38" s="2" t="n"/>
-      <c r="S38" s="2" t="inlineStr">
+      <c r="G39" s="2" t="n"/>
+      <c r="H39" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I39" s="2" t="n"/>
+      <c r="J39" s="2" t="n"/>
+      <c r="K39" s="2" t="n"/>
+      <c r="L39" s="2" t="n"/>
+      <c r="M39" s="2" t="n"/>
+      <c r="N39" s="2" t="n"/>
+      <c r="O39" s="2" t="n"/>
+      <c r="P39" s="2" t="n"/>
+      <c r="Q39" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R39" s="2" t="n"/>
+      <c r="S39" s="2" t="inlineStr">
         <is>
           <t>JH; RW</t>
         </is>
       </c>
-      <c r="T38" s="2" t="inlineStr">
-        <is>
-          <t>Published</t>
-        </is>
-      </c>
-      <c r="U38" s="2" t="n"/>
-      <c r="V38" s="2" t="n"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="3" t="inlineStr">
-        <is>
-          <t>BCIO:050462</t>
-        </is>
-      </c>
-      <c r="B39" s="3" t="inlineStr">
-        <is>
-          <t>high cognitive exertion expended on a behaviour</t>
-        </is>
-      </c>
-      <c r="C39" s="3" t="inlineStr">
-        <is>
-          <t>Cognitive exertion expended on a behaviour that is high.</t>
-        </is>
-      </c>
-      <c r="D39" s="3" t="n"/>
-      <c r="E39" s="3" t="n"/>
-      <c r="F39" s="3" t="n"/>
-      <c r="G39" s="3" t="inlineStr">
-        <is>
-          <t>cognitive exertion expended on a behaviour</t>
-        </is>
-      </c>
-      <c r="H39" s="3" t="n"/>
-      <c r="I39" s="3" t="inlineStr">
-        <is>
-          <t>behaviour</t>
-        </is>
-      </c>
-      <c r="J39" s="3" t="n"/>
-      <c r="K39" s="3" t="n"/>
-      <c r="L39" s="3" t="n"/>
-      <c r="M39" s="3" t="n"/>
-      <c r="N39" s="3" t="n"/>
-      <c r="O39" s="3" t="inlineStr">
-        <is>
-          <t>High cognitive exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what high exertion means based on the measurement you use).</t>
-        </is>
-      </c>
-      <c r="P39" s="3" t="n"/>
-      <c r="Q39" s="3" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="R39" s="3" t="n"/>
-      <c r="S39" s="3" t="inlineStr">
-        <is>
-          <t>PS</t>
-        </is>
-      </c>
-      <c r="T39" s="3" t="inlineStr">
-        <is>
-          <t>Obsolete</t>
-        </is>
-      </c>
-      <c r="U39" s="3" t="n"/>
-      <c r="V39" s="3" t="n"/>
+      <c r="T39" s="2" t="inlineStr">
+        <is>
+          <t>Published</t>
+        </is>
+      </c>
+      <c r="U39" s="2" t="n"/>
+      <c r="V39" s="2" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>BCIO:050463</t>
+          <t>BCIO:050462</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>high emotional management  exertion expended on a behaviour</t>
+          <t>high cognitive exertion expended on a behaviour</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
         <is>
-          <t>Emotional management exertion expended on a behaviour that is high.</t>
+          <t>Cognitive exertion expended on a behaviour that is high.</t>
         </is>
       </c>
       <c r="D40" s="3" t="n"/>
       <c r="E40" s="3" t="n"/>
-      <c r="F40" s="3" t="n"/>
-      <c r="G40" s="3" t="inlineStr">
-        <is>
-          <t>emotional management exertion expended on a behaviour</t>
-        </is>
-      </c>
-      <c r="H40" s="3" t="n"/>
-      <c r="I40" s="3" t="inlineStr">
+      <c r="F40" s="3" t="inlineStr">
+        <is>
+          <t>cognitive exertion expended on a behaviour</t>
+        </is>
+      </c>
+      <c r="G40" s="3" t="n"/>
+      <c r="H40" s="3" t="inlineStr">
         <is>
           <t>behaviour</t>
         </is>
       </c>
+      <c r="I40" s="3" t="n"/>
       <c r="J40" s="3" t="n"/>
       <c r="K40" s="3" t="n"/>
       <c r="L40" s="3" t="n"/>
@@ -3003,7 +2981,7 @@
       <c r="N40" s="3" t="n"/>
       <c r="O40" s="3" t="inlineStr">
         <is>
-          <t>High emotional management exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what high exertion means based on the measurement you use).</t>
+          <t>High cognitive exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what high exertion means based on the measurement you use).</t>
         </is>
       </c>
       <c r="P40" s="3" t="n"/>
@@ -3029,33 +3007,33 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>BCIO:050464</t>
+          <t>BCIO:050463</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>high mental exertion expended on a behaviour</t>
+          <t>high emotional management  exertion expended on a behaviour</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
         <is>
-          <t>Mental exertion expended on a behaviour that is high.</t>
+          <t>Emotional management exertion expended on a behaviour that is high.</t>
         </is>
       </c>
       <c r="D41" s="3" t="n"/>
       <c r="E41" s="3" t="n"/>
-      <c r="F41" s="3" t="n"/>
-      <c r="G41" s="3" t="inlineStr">
-        <is>
-          <t>mental exertion expended on a behaviour</t>
-        </is>
-      </c>
-      <c r="H41" s="3" t="n"/>
-      <c r="I41" s="3" t="inlineStr">
+      <c r="F41" s="3" t="inlineStr">
+        <is>
+          <t>emotional management exertion expended on a behaviour</t>
+        </is>
+      </c>
+      <c r="G41" s="3" t="n"/>
+      <c r="H41" s="3" t="inlineStr">
         <is>
           <t>behaviour</t>
         </is>
       </c>
+      <c r="I41" s="3" t="n"/>
       <c r="J41" s="3" t="n"/>
       <c r="K41" s="3" t="n"/>
       <c r="L41" s="3" t="n"/>
@@ -3063,7 +3041,7 @@
       <c r="N41" s="3" t="n"/>
       <c r="O41" s="3" t="inlineStr">
         <is>
-          <t>High mental exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what high exertion means based on the measurement you use).</t>
+          <t>High emotional management exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what high exertion means based on the measurement you use).</t>
         </is>
       </c>
       <c r="P41" s="3" t="n"/>
@@ -3089,33 +3067,33 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>BCIO:050465</t>
+          <t>BCIO:050464</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>high physical exertion expended on behaviour</t>
+          <t>high mental exertion expended on a behaviour</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
         <is>
-          <t>Physical exertion expended on a behaviour that is high</t>
+          <t>Mental exertion expended on a behaviour that is high.</t>
         </is>
       </c>
       <c r="D42" s="3" t="n"/>
       <c r="E42" s="3" t="n"/>
-      <c r="F42" s="3" t="n"/>
-      <c r="G42" s="3" t="inlineStr">
-        <is>
-          <t>physical exertion expended on a behaviour</t>
-        </is>
-      </c>
-      <c r="H42" s="3" t="n"/>
-      <c r="I42" s="3" t="inlineStr">
+      <c r="F42" s="3" t="inlineStr">
+        <is>
+          <t>mental exertion expended on a behaviour</t>
+        </is>
+      </c>
+      <c r="G42" s="3" t="n"/>
+      <c r="H42" s="3" t="inlineStr">
         <is>
           <t>behaviour</t>
         </is>
       </c>
+      <c r="I42" s="3" t="n"/>
       <c r="J42" s="3" t="n"/>
       <c r="K42" s="3" t="n"/>
       <c r="L42" s="3" t="n"/>
@@ -3123,7 +3101,7 @@
       <c r="N42" s="3" t="n"/>
       <c r="O42" s="3" t="inlineStr">
         <is>
-          <t>High physical exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what high exertion means based on the measurement you use).</t>
+          <t>High mental exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what high exertion means based on the measurement you use).</t>
         </is>
       </c>
       <c r="P42" s="3" t="n"/>
@@ -3147,95 +3125,99 @@
       <c r="V42" s="3" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="2" t="inlineStr">
-        <is>
-          <t>BCIO:042000</t>
-        </is>
-      </c>
-      <c r="B43" s="2" t="inlineStr">
-        <is>
-          <t>human behaviour</t>
-        </is>
-      </c>
-      <c r="C43" s="2" t="inlineStr">
-        <is>
-          <t>A process that is an individual human behaviour or a population behaviour.</t>
-        </is>
-      </c>
-      <c r="D43" s="2" t="n"/>
-      <c r="E43" s="2" t="inlineStr">
-        <is>
-          <t>"individual human behaviour" OR "population behaviour"</t>
-        </is>
-      </c>
-      <c r="F43" s="2" t="n"/>
-      <c r="G43" s="2" t="inlineStr">
-        <is>
-          <t>process</t>
-        </is>
-      </c>
-      <c r="H43" s="2" t="n"/>
-      <c r="I43" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
-      <c r="J43" s="2" t="n"/>
-      <c r="K43" s="2" t="n"/>
-      <c r="L43" s="2" t="n"/>
-      <c r="M43" s="2" t="n"/>
-      <c r="N43" s="2" t="n"/>
-      <c r="O43" s="2" t="n"/>
-      <c r="P43" s="2" t="n"/>
-      <c r="Q43" s="2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="R43" s="2" t="n"/>
-      <c r="S43" s="2" t="inlineStr">
-        <is>
-          <t>BG; PS</t>
-        </is>
-      </c>
-      <c r="T43" s="2" t="inlineStr">
-        <is>
-          <t>Published</t>
-        </is>
-      </c>
-      <c r="U43" s="2" t="n"/>
-      <c r="V43" s="2" t="n"/>
+      <c r="A43" s="3" t="inlineStr">
+        <is>
+          <t>BCIO:050465</t>
+        </is>
+      </c>
+      <c r="B43" s="3" t="inlineStr">
+        <is>
+          <t>high physical exertion expended on behaviour</t>
+        </is>
+      </c>
+      <c r="C43" s="3" t="inlineStr">
+        <is>
+          <t>Physical exertion expended on a behaviour that is high</t>
+        </is>
+      </c>
+      <c r="D43" s="3" t="n"/>
+      <c r="E43" s="3" t="n"/>
+      <c r="F43" s="3" t="inlineStr">
+        <is>
+          <t>physical exertion expended on a behaviour</t>
+        </is>
+      </c>
+      <c r="G43" s="3" t="n"/>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
+          <t>behaviour</t>
+        </is>
+      </c>
+      <c r="I43" s="3" t="n"/>
+      <c r="J43" s="3" t="n"/>
+      <c r="K43" s="3" t="n"/>
+      <c r="L43" s="3" t="n"/>
+      <c r="M43" s="3" t="n"/>
+      <c r="N43" s="3" t="n"/>
+      <c r="O43" s="3" t="inlineStr">
+        <is>
+          <t>High physical exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what high exertion means based on the measurement you use).</t>
+        </is>
+      </c>
+      <c r="P43" s="3" t="n"/>
+      <c r="Q43" s="3" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R43" s="3" t="n"/>
+      <c r="S43" s="3" t="inlineStr">
+        <is>
+          <t>PS</t>
+        </is>
+      </c>
+      <c r="T43" s="3" t="inlineStr">
+        <is>
+          <t>Obsolete</t>
+        </is>
+      </c>
+      <c r="U43" s="3" t="n"/>
+      <c r="V43" s="3" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>BCIO:041000</t>
+          <t>BCIO:042000</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>human population</t>
+          <t>human behaviour</t>
         </is>
       </c>
       <c r="C44" s="2" t="inlineStr">
         <is>
-          <t>An object aggregate that consists of two or more people.</t>
+          <t>A process that is an individual human behaviour or a population behaviour.</t>
         </is>
       </c>
       <c r="D44" s="2" t="n"/>
-      <c r="E44" s="2" t="n"/>
-      <c r="F44" s="2" t="n"/>
-      <c r="G44" s="2" t="inlineStr">
-        <is>
-          <t>object aggregate</t>
-        </is>
-      </c>
-      <c r="H44" s="2" t="n"/>
-      <c r="I44" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="E44" s="2" t="inlineStr">
+        <is>
+          <t>"individual human behaviour" OR "population behaviour"</t>
+        </is>
+      </c>
+      <c r="F44" s="2" t="inlineStr">
+        <is>
+          <t>process</t>
+        </is>
+      </c>
+      <c r="G44" s="2" t="n"/>
+      <c r="H44" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I44" s="2" t="n"/>
       <c r="J44" s="2" t="n"/>
       <c r="K44" s="2" t="n"/>
       <c r="L44" s="2" t="n"/>
@@ -3251,7 +3233,7 @@
       <c r="R44" s="2" t="n"/>
       <c r="S44" s="2" t="inlineStr">
         <is>
-          <t>JH; AW</t>
+          <t>BG; PS</t>
         </is>
       </c>
       <c r="T44" s="2" t="inlineStr">
@@ -3265,33 +3247,33 @@
     <row r="45">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>BCIO:040000</t>
+          <t>BCIO:041000</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
         <is>
-          <t>individual human activity</t>
+          <t>human population</t>
         </is>
       </c>
       <c r="C45" s="2" t="inlineStr">
         <is>
-          <t>A process that is produced by a person.</t>
+          <t>An object aggregate that consists of two or more people.</t>
         </is>
       </c>
       <c r="D45" s="2" t="n"/>
       <c r="E45" s="2" t="n"/>
-      <c r="F45" s="2" t="n"/>
-      <c r="G45" s="2" t="inlineStr">
-        <is>
-          <t>process</t>
-        </is>
-      </c>
-      <c r="H45" s="2" t="n"/>
-      <c r="I45" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="F45" s="2" t="inlineStr">
+        <is>
+          <t>object aggregate</t>
+        </is>
+      </c>
+      <c r="G45" s="2" t="n"/>
+      <c r="H45" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I45" s="2" t="n"/>
       <c r="J45" s="2" t="n"/>
       <c r="K45" s="2" t="n"/>
       <c r="L45" s="2" t="n"/>
@@ -3307,7 +3289,7 @@
       <c r="R45" s="2" t="n"/>
       <c r="S45" s="2" t="inlineStr">
         <is>
-          <t>JH</t>
+          <t>JH; AW</t>
         </is>
       </c>
       <c r="T45" s="2" t="inlineStr">
@@ -3321,48 +3303,40 @@
     <row r="46">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>BCIO:036000</t>
+          <t>BCIO:040000</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
-          <t>individual human behaviour</t>
+          <t>individual human activity</t>
         </is>
       </c>
       <c r="C46" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">A bodily process of a human that involves co-ordinated contraction of striated muscles controlled by the brain. </t>
+          <t>A process that is produced by a person.</t>
         </is>
       </c>
       <c r="D46" s="2" t="n"/>
       <c r="E46" s="2" t="n"/>
-      <c r="F46" s="2" t="n"/>
-      <c r="G46" s="2" t="inlineStr">
-        <is>
-          <t>bodily process</t>
-        </is>
-      </c>
-      <c r="H46" s="2" t="n"/>
-      <c r="I46" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="F46" s="2" t="inlineStr">
+        <is>
+          <t>process</t>
+        </is>
+      </c>
+      <c r="G46" s="2" t="n"/>
+      <c r="H46" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I46" s="2" t="n"/>
       <c r="J46" s="2" t="n"/>
       <c r="K46" s="2" t="n"/>
       <c r="L46" s="2" t="n"/>
-      <c r="M46" s="2" t="inlineStr">
-        <is>
-          <t>human behaviour</t>
-        </is>
-      </c>
+      <c r="M46" s="2" t="n"/>
       <c r="N46" s="2" t="n"/>
       <c r="O46" s="2" t="n"/>
-      <c r="P46" s="2" t="inlineStr">
-        <is>
-          <t>Also referred to in definitions as human behaviour or just behaviour.</t>
-        </is>
-      </c>
+      <c r="P46" s="2" t="n"/>
       <c r="Q46" s="2" t="inlineStr">
         <is>
           <t>0</t>
@@ -3385,42 +3359,46 @@
     <row r="47">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>BCIO:037000</t>
+          <t>BCIO:036000</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
         <is>
-          <t>intervention</t>
+          <t>individual human behaviour</t>
         </is>
       </c>
       <c r="C47" s="2" t="inlineStr">
         <is>
-          <t>A planned process that has the aim of influencing an outcome.</t>
+          <t xml:space="preserve">A bodily process of a human that involves co-ordinated contraction of striated muscles controlled by the brain. </t>
         </is>
       </c>
       <c r="D47" s="2" t="n"/>
       <c r="E47" s="2" t="n"/>
-      <c r="F47" s="2" t="n"/>
-      <c r="G47" s="2" t="inlineStr">
-        <is>
-          <t>planned process</t>
-        </is>
-      </c>
-      <c r="H47" s="2" t="n"/>
-      <c r="I47" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="F47" s="2" t="inlineStr">
+        <is>
+          <t>bodily process</t>
+        </is>
+      </c>
+      <c r="G47" s="2" t="n"/>
+      <c r="H47" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I47" s="2" t="n"/>
       <c r="J47" s="2" t="n"/>
       <c r="K47" s="2" t="n"/>
       <c r="L47" s="2" t="n"/>
-      <c r="M47" s="2" t="n"/>
+      <c r="M47" s="2" t="inlineStr">
+        <is>
+          <t>human behaviour</t>
+        </is>
+      </c>
       <c r="N47" s="2" t="n"/>
       <c r="O47" s="2" t="n"/>
       <c r="P47" s="2" t="inlineStr">
         <is>
-          <t>Examples of interventions are putting health warnings on cigarette packets, providing free stop smoking services and banning smoking in public places.</t>
+          <t>Also referred to in definitions as human behaviour or just behaviour.</t>
         </is>
       </c>
       <c r="Q47" s="2" t="inlineStr">
@@ -3431,7 +3409,7 @@
       <c r="R47" s="2" t="n"/>
       <c r="S47" s="2" t="inlineStr">
         <is>
-          <t>JH; RW</t>
+          <t>JH</t>
         </is>
       </c>
       <c r="T47" s="2" t="inlineStr">
@@ -3445,40 +3423,44 @@
     <row r="48">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>BCIO:046000</t>
+          <t>BCIO:037000</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
         <is>
-          <t>intervention content</t>
+          <t>intervention</t>
         </is>
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
-          <t>A planned process that is part of an intervention and is intended to be causally active in influencing the intervention outcome.</t>
+          <t>A planned process that has the aim of influencing an outcome.</t>
         </is>
       </c>
       <c r="D48" s="2" t="n"/>
       <c r="E48" s="2" t="n"/>
-      <c r="F48" s="2" t="n"/>
-      <c r="G48" s="2" t="inlineStr">
+      <c r="F48" s="2" t="inlineStr">
         <is>
           <t>planned process</t>
         </is>
       </c>
-      <c r="H48" s="2" t="n"/>
-      <c r="I48" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G48" s="2" t="n"/>
+      <c r="H48" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I48" s="2" t="n"/>
       <c r="J48" s="2" t="n"/>
       <c r="K48" s="2" t="n"/>
       <c r="L48" s="2" t="n"/>
       <c r="M48" s="2" t="n"/>
       <c r="N48" s="2" t="n"/>
       <c r="O48" s="2" t="n"/>
-      <c r="P48" s="2" t="n"/>
+      <c r="P48" s="2" t="inlineStr">
+        <is>
+          <t>Examples of interventions are putting health warnings on cigarette packets, providing free stop smoking services and banning smoking in public places.</t>
+        </is>
+      </c>
       <c r="Q48" s="2" t="inlineStr">
         <is>
           <t>0</t>
@@ -3487,7 +3469,7 @@
       <c r="R48" s="2" t="n"/>
       <c r="S48" s="2" t="inlineStr">
         <is>
-          <t>RW</t>
+          <t>JH; RW</t>
         </is>
       </c>
       <c r="T48" s="2" t="inlineStr">
@@ -3501,33 +3483,33 @@
     <row r="49">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>BCIO:045000</t>
+          <t>BCIO:046000</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
         <is>
-          <t>intervention delivery</t>
+          <t>intervention content</t>
         </is>
       </c>
       <c r="C49" s="2" t="inlineStr">
         <is>
-          <t>A planned process by which intervention content is delivered.</t>
+          <t>A planned process that is part of an intervention and is intended to be causally active in influencing the intervention outcome.</t>
         </is>
       </c>
       <c r="D49" s="2" t="n"/>
       <c r="E49" s="2" t="n"/>
-      <c r="F49" s="2" t="n"/>
-      <c r="G49" s="2" t="inlineStr">
+      <c r="F49" s="2" t="inlineStr">
         <is>
           <t>planned process</t>
         </is>
       </c>
-      <c r="H49" s="2" t="n"/>
-      <c r="I49" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="G49" s="2" t="n"/>
+      <c r="H49" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I49" s="2" t="n"/>
       <c r="J49" s="2" t="n"/>
       <c r="K49" s="2" t="n"/>
       <c r="L49" s="2" t="n"/>
@@ -3557,33 +3539,33 @@
     <row r="50">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>BCIO:038000</t>
+          <t>BCIO:045000</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
         <is>
-          <t>intervention evaluation study</t>
+          <t>intervention delivery</t>
         </is>
       </c>
       <c r="C50" s="2" t="inlineStr">
         <is>
-          <t>A research study that aims to assess attributes of an intervention with regards to their positive or negative value.</t>
+          <t>A planned process by which intervention content is delivered.</t>
         </is>
       </c>
       <c r="D50" s="2" t="n"/>
       <c r="E50" s="2" t="n"/>
-      <c r="F50" s="2" t="n"/>
-      <c r="G50" s="2" t="inlineStr">
-        <is>
-          <t>research study</t>
-        </is>
-      </c>
-      <c r="H50" s="2" t="n"/>
-      <c r="I50" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="F50" s="2" t="inlineStr">
+        <is>
+          <t>planned process</t>
+        </is>
+      </c>
+      <c r="G50" s="2" t="n"/>
+      <c r="H50" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I50" s="2" t="n"/>
       <c r="J50" s="2" t="n"/>
       <c r="K50" s="2" t="n"/>
       <c r="L50" s="2" t="n"/>
@@ -3599,7 +3581,7 @@
       <c r="R50" s="2" t="n"/>
       <c r="S50" s="2" t="inlineStr">
         <is>
-          <t>JH; RW</t>
+          <t>RW</t>
         </is>
       </c>
       <c r="T50" s="2" t="inlineStr">
@@ -3613,44 +3595,40 @@
     <row r="51">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>BCIO:039000</t>
+          <t>BCIO:038000</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
         <is>
-          <t>intervention outcome</t>
+          <t>intervention evaluation study</t>
         </is>
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>A process that is influenced by an intervention.</t>
+          <t>A research study that aims to assess attributes of an intervention with regards to their positive or negative value.</t>
         </is>
       </c>
       <c r="D51" s="2" t="n"/>
       <c r="E51" s="2" t="n"/>
-      <c r="F51" s="2" t="n"/>
-      <c r="G51" s="2" t="inlineStr">
-        <is>
-          <t>process</t>
-        </is>
-      </c>
-      <c r="H51" s="2" t="n"/>
-      <c r="I51" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="F51" s="2" t="inlineStr">
+        <is>
+          <t>research study</t>
+        </is>
+      </c>
+      <c r="G51" s="2" t="n"/>
+      <c r="H51" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I51" s="2" t="n"/>
       <c r="J51" s="2" t="n"/>
       <c r="K51" s="2" t="n"/>
       <c r="L51" s="2" t="n"/>
       <c r="M51" s="2" t="n"/>
       <c r="N51" s="2" t="n"/>
       <c r="O51" s="2" t="n"/>
-      <c r="P51" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Includes individual human behaviour, mental activity and physiological activity. Also includes undesirable outcomes, such as treatment side effects, and unintended negative consequences of the intervention. </t>
-        </is>
-      </c>
+      <c r="P51" s="2" t="n"/>
       <c r="Q51" s="2" t="inlineStr">
         <is>
           <t>0</t>
@@ -3659,7 +3637,7 @@
       <c r="R51" s="2" t="n"/>
       <c r="S51" s="2" t="inlineStr">
         <is>
-          <t>JH</t>
+          <t>JH; RW</t>
         </is>
       </c>
       <c r="T51" s="2" t="inlineStr">
@@ -3673,40 +3651,44 @@
     <row r="52">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>BCIO:015095</t>
+          <t>BCIO:039000</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
         <is>
-          <t>intervention population</t>
+          <t>intervention outcome</t>
         </is>
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>A human population who are exposed to an intervention.</t>
+          <t>A process that is influenced by an intervention.</t>
         </is>
       </c>
       <c r="D52" s="2" t="n"/>
       <c r="E52" s="2" t="n"/>
-      <c r="F52" s="2" t="n"/>
-      <c r="G52" s="2" t="inlineStr">
-        <is>
-          <t>human population</t>
-        </is>
-      </c>
-      <c r="H52" s="2" t="n"/>
-      <c r="I52" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="F52" s="2" t="inlineStr">
+        <is>
+          <t>process</t>
+        </is>
+      </c>
+      <c r="G52" s="2" t="n"/>
+      <c r="H52" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I52" s="2" t="n"/>
       <c r="J52" s="2" t="n"/>
       <c r="K52" s="2" t="n"/>
       <c r="L52" s="2" t="n"/>
       <c r="M52" s="2" t="n"/>
       <c r="N52" s="2" t="n"/>
       <c r="O52" s="2" t="n"/>
-      <c r="P52" s="2" t="n"/>
+      <c r="P52" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Includes individual human behaviour, mental activity and physiological activity. Also includes undesirable outcomes, such as treatment side effects, and unintended negative consequences of the intervention. </t>
+        </is>
+      </c>
       <c r="Q52" s="2" t="inlineStr">
         <is>
           <t>0</t>
@@ -3715,7 +3697,7 @@
       <c r="R52" s="2" t="n"/>
       <c r="S52" s="2" t="inlineStr">
         <is>
-          <t>AW; PS</t>
+          <t>JH</t>
         </is>
       </c>
       <c r="T52" s="2" t="inlineStr">
@@ -3727,95 +3709,91 @@
       <c r="V52" s="2" t="n"/>
     </row>
     <row r="53">
-      <c r="A53" s="3" t="inlineStr">
-        <is>
-          <t>BCIO:050466</t>
-        </is>
-      </c>
-      <c r="B53" s="3" t="inlineStr">
-        <is>
-          <t>low cognitive exertion expended on a behaviour</t>
-        </is>
-      </c>
-      <c r="C53" s="3" t="inlineStr">
-        <is>
-          <t>Cognitive exertion expended on a behaviour that is low.</t>
-        </is>
-      </c>
-      <c r="D53" s="3" t="n"/>
-      <c r="E53" s="3" t="n"/>
-      <c r="F53" s="3" t="n"/>
-      <c r="G53" s="3" t="inlineStr">
-        <is>
-          <t>cognitive exertion expended on a behaviour</t>
-        </is>
-      </c>
-      <c r="H53" s="3" t="n"/>
-      <c r="I53" s="3" t="inlineStr">
-        <is>
-          <t>behaviour</t>
-        </is>
-      </c>
-      <c r="J53" s="3" t="n"/>
-      <c r="K53" s="3" t="n"/>
-      <c r="L53" s="3" t="n"/>
-      <c r="M53" s="3" t="n"/>
-      <c r="N53" s="3" t="n"/>
-      <c r="O53" s="3" t="inlineStr">
-        <is>
-          <t>Low cognitive exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what low exertion means based on the measurement you use).</t>
-        </is>
-      </c>
-      <c r="P53" s="3" t="n"/>
-      <c r="Q53" s="3" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="R53" s="3" t="n"/>
-      <c r="S53" s="3" t="inlineStr">
-        <is>
-          <t>PS</t>
-        </is>
-      </c>
-      <c r="T53" s="3" t="inlineStr">
-        <is>
-          <t>Obsolete</t>
-        </is>
-      </c>
-      <c r="U53" s="3" t="n"/>
-      <c r="V53" s="3" t="n"/>
+      <c r="A53" s="2" t="inlineStr">
+        <is>
+          <t>BCIO:015095</t>
+        </is>
+      </c>
+      <c r="B53" s="2" t="inlineStr">
+        <is>
+          <t>intervention population</t>
+        </is>
+      </c>
+      <c r="C53" s="2" t="inlineStr">
+        <is>
+          <t>A human population who are exposed to an intervention.</t>
+        </is>
+      </c>
+      <c r="D53" s="2" t="n"/>
+      <c r="E53" s="2" t="n"/>
+      <c r="F53" s="2" t="inlineStr">
+        <is>
+          <t>human population</t>
+        </is>
+      </c>
+      <c r="G53" s="2" t="n"/>
+      <c r="H53" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I53" s="2" t="n"/>
+      <c r="J53" s="2" t="n"/>
+      <c r="K53" s="2" t="n"/>
+      <c r="L53" s="2" t="n"/>
+      <c r="M53" s="2" t="n"/>
+      <c r="N53" s="2" t="n"/>
+      <c r="O53" s="2" t="n"/>
+      <c r="P53" s="2" t="n"/>
+      <c r="Q53" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R53" s="2" t="n"/>
+      <c r="S53" s="2" t="inlineStr">
+        <is>
+          <t>AW; PS</t>
+        </is>
+      </c>
+      <c r="T53" s="2" t="inlineStr">
+        <is>
+          <t>Published</t>
+        </is>
+      </c>
+      <c r="U53" s="2" t="n"/>
+      <c r="V53" s="2" t="n"/>
     </row>
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>BCIO:050467</t>
+          <t>BCIO:050466</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>low emotional management exertion expended on a behaviour</t>
+          <t>low cognitive exertion expended on a behaviour</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
         <is>
-          <t>Emotional management exertion expended on a behaviour that is low.</t>
+          <t>Cognitive exertion expended on a behaviour that is low.</t>
         </is>
       </c>
       <c r="D54" s="3" t="n"/>
       <c r="E54" s="3" t="n"/>
-      <c r="F54" s="3" t="n"/>
-      <c r="G54" s="3" t="inlineStr">
-        <is>
-          <t>emotional management exertion expended on a behaviour</t>
-        </is>
-      </c>
-      <c r="H54" s="3" t="n"/>
-      <c r="I54" s="3" t="inlineStr">
+      <c r="F54" s="3" t="inlineStr">
+        <is>
+          <t>cognitive exertion expended on a behaviour</t>
+        </is>
+      </c>
+      <c r="G54" s="3" t="n"/>
+      <c r="H54" s="3" t="inlineStr">
         <is>
           <t>behaviour</t>
         </is>
       </c>
+      <c r="I54" s="3" t="n"/>
       <c r="J54" s="3" t="n"/>
       <c r="K54" s="3" t="n"/>
       <c r="L54" s="3" t="n"/>
@@ -3823,7 +3801,7 @@
       <c r="N54" s="3" t="n"/>
       <c r="O54" s="3" t="inlineStr">
         <is>
-          <t>Low emotional management exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what low exertion means based on the measurement you use).</t>
+          <t>Low cognitive exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what low exertion means based on the measurement you use).</t>
         </is>
       </c>
       <c r="P54" s="3" t="n"/>
@@ -3849,33 +3827,33 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>BCIO:050468</t>
+          <t>BCIO:050467</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>low mental exertion expended on a behaviour</t>
+          <t>low emotional management exertion expended on a behaviour</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr">
         <is>
-          <t>Mental exertion expended on a behaviour that is low.</t>
+          <t>Emotional management exertion expended on a behaviour that is low.</t>
         </is>
       </c>
       <c r="D55" s="3" t="n"/>
       <c r="E55" s="3" t="n"/>
-      <c r="F55" s="3" t="n"/>
-      <c r="G55" s="3" t="inlineStr">
-        <is>
-          <t>mental exertion expended on a behaviour</t>
-        </is>
-      </c>
-      <c r="H55" s="3" t="n"/>
-      <c r="I55" s="3" t="inlineStr">
+      <c r="F55" s="3" t="inlineStr">
+        <is>
+          <t>emotional management exertion expended on a behaviour</t>
+        </is>
+      </c>
+      <c r="G55" s="3" t="n"/>
+      <c r="H55" s="3" t="inlineStr">
         <is>
           <t>behaviour</t>
         </is>
       </c>
+      <c r="I55" s="3" t="n"/>
       <c r="J55" s="3" t="n"/>
       <c r="K55" s="3" t="n"/>
       <c r="L55" s="3" t="n"/>
@@ -3883,7 +3861,7 @@
       <c r="N55" s="3" t="n"/>
       <c r="O55" s="3" t="inlineStr">
         <is>
-          <t>Low mental exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what low exertion means based on the measurement you use).</t>
+          <t>Low emotional management exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what low exertion means based on the measurement you use).</t>
         </is>
       </c>
       <c r="P55" s="3" t="n"/>
@@ -3909,33 +3887,33 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>BCIO:050469</t>
+          <t>BCIO:050468</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
         <is>
-          <t>low physical exertion expended on behaviour</t>
+          <t>low mental exertion expended on a behaviour</t>
         </is>
       </c>
       <c r="C56" s="3" t="inlineStr">
         <is>
-          <t>Physical exertion expended on a behaviour that is low.</t>
+          <t>Mental exertion expended on a behaviour that is low.</t>
         </is>
       </c>
       <c r="D56" s="3" t="n"/>
       <c r="E56" s="3" t="n"/>
-      <c r="F56" s="3" t="n"/>
-      <c r="G56" s="3" t="inlineStr">
-        <is>
-          <t>physical exertion expended on a behaviour</t>
-        </is>
-      </c>
-      <c r="H56" s="3" t="n"/>
-      <c r="I56" s="3" t="inlineStr">
+      <c r="F56" s="3" t="inlineStr">
+        <is>
+          <t>mental exertion expended on a behaviour</t>
+        </is>
+      </c>
+      <c r="G56" s="3" t="n"/>
+      <c r="H56" s="3" t="inlineStr">
         <is>
           <t>behaviour</t>
         </is>
       </c>
+      <c r="I56" s="3" t="n"/>
       <c r="J56" s="3" t="n"/>
       <c r="K56" s="3" t="n"/>
       <c r="L56" s="3" t="n"/>
@@ -3943,7 +3921,7 @@
       <c r="N56" s="3" t="n"/>
       <c r="O56" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Low physical exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what low exertion means </t>
+          <t>Low mental exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what low exertion means based on the measurement you use).</t>
         </is>
       </c>
       <c r="P56" s="3" t="n"/>
@@ -3969,33 +3947,33 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>BCIO:050470</t>
+          <t>BCIO:050469</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>moderate cognitive exertion expended on a behaviour</t>
+          <t>low physical exertion expended on behaviour</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
         <is>
-          <t>Cognitive exertion expended on a behaviour that is medium.</t>
+          <t>Physical exertion expended on a behaviour that is low.</t>
         </is>
       </c>
       <c r="D57" s="3" t="n"/>
       <c r="E57" s="3" t="n"/>
-      <c r="F57" s="3" t="n"/>
-      <c r="G57" s="3" t="inlineStr">
-        <is>
-          <t>cognitive exertion expended on a behaviour</t>
-        </is>
-      </c>
-      <c r="H57" s="3" t="n"/>
-      <c r="I57" s="3" t="inlineStr">
+      <c r="F57" s="3" t="inlineStr">
+        <is>
+          <t>physical exertion expended on a behaviour</t>
+        </is>
+      </c>
+      <c r="G57" s="3" t="n"/>
+      <c r="H57" s="3" t="inlineStr">
         <is>
           <t>behaviour</t>
         </is>
       </c>
+      <c r="I57" s="3" t="n"/>
       <c r="J57" s="3" t="n"/>
       <c r="K57" s="3" t="n"/>
       <c r="L57" s="3" t="n"/>
@@ -4003,7 +3981,7 @@
       <c r="N57" s="3" t="n"/>
       <c r="O57" s="3" t="inlineStr">
         <is>
-          <t>Moderate cognitive exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what moderate exertion means based on the measurement you use).</t>
+          <t xml:space="preserve">Low physical exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what low exertion means </t>
         </is>
       </c>
       <c r="P57" s="3" t="n"/>
@@ -4029,33 +4007,33 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>BCIO:050471</t>
+          <t>BCIO:050470</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>moderate emotional management exertion expended on a behaviour</t>
+          <t>moderate cognitive exertion expended on a behaviour</t>
         </is>
       </c>
       <c r="C58" s="3" t="inlineStr">
         <is>
-          <t>Emotional management exertion expended on a behaviour that is medium.</t>
+          <t>Cognitive exertion expended on a behaviour that is medium.</t>
         </is>
       </c>
       <c r="D58" s="3" t="n"/>
       <c r="E58" s="3" t="n"/>
-      <c r="F58" s="3" t="n"/>
-      <c r="G58" s="3" t="inlineStr">
-        <is>
-          <t>emotional management exertion expended on a behaviour</t>
-        </is>
-      </c>
-      <c r="H58" s="3" t="n"/>
-      <c r="I58" s="3" t="inlineStr">
+      <c r="F58" s="3" t="inlineStr">
+        <is>
+          <t>cognitive exertion expended on a behaviour</t>
+        </is>
+      </c>
+      <c r="G58" s="3" t="n"/>
+      <c r="H58" s="3" t="inlineStr">
         <is>
           <t>behaviour</t>
         </is>
       </c>
+      <c r="I58" s="3" t="n"/>
       <c r="J58" s="3" t="n"/>
       <c r="K58" s="3" t="n"/>
       <c r="L58" s="3" t="n"/>
@@ -4063,7 +4041,7 @@
       <c r="N58" s="3" t="n"/>
       <c r="O58" s="3" t="inlineStr">
         <is>
-          <t>Moderate emotional management exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what moderate exertion means based on the measurement you use).</t>
+          <t>Moderate cognitive exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what moderate exertion means based on the measurement you use).</t>
         </is>
       </c>
       <c r="P58" s="3" t="n"/>
@@ -4089,33 +4067,33 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>BCIO:050472</t>
+          <t>BCIO:050471</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>moderate mental exertion expended on a behaviour</t>
+          <t>moderate emotional management exertion expended on a behaviour</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr">
         <is>
-          <t>Mental exertion expended on a behaviour that is medium.</t>
+          <t>Emotional management exertion expended on a behaviour that is medium.</t>
         </is>
       </c>
       <c r="D59" s="3" t="n"/>
       <c r="E59" s="3" t="n"/>
-      <c r="F59" s="3" t="n"/>
-      <c r="G59" s="3" t="inlineStr">
-        <is>
-          <t>mental exertion expended on a behaviour</t>
-        </is>
-      </c>
-      <c r="H59" s="3" t="n"/>
-      <c r="I59" s="3" t="inlineStr">
+      <c r="F59" s="3" t="inlineStr">
+        <is>
+          <t>emotional management exertion expended on a behaviour</t>
+        </is>
+      </c>
+      <c r="G59" s="3" t="n"/>
+      <c r="H59" s="3" t="inlineStr">
         <is>
           <t>behaviour</t>
         </is>
       </c>
+      <c r="I59" s="3" t="n"/>
       <c r="J59" s="3" t="n"/>
       <c r="K59" s="3" t="n"/>
       <c r="L59" s="3" t="n"/>
@@ -4123,7 +4101,7 @@
       <c r="N59" s="3" t="n"/>
       <c r="O59" s="3" t="inlineStr">
         <is>
-          <t>Moderate mental exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what moderate exertion means based on the measurement you use).</t>
+          <t>Moderate emotional management exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what moderate exertion means based on the measurement you use).</t>
         </is>
       </c>
       <c r="P59" s="3" t="n"/>
@@ -4149,33 +4127,33 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>BCIO:050473</t>
+          <t>BCIO:050472</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t>moderate physical exertion expended on behaviour</t>
+          <t>moderate mental exertion expended on a behaviour</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr">
         <is>
-          <t>Physical exertion expended on a behaviour that is medium.</t>
+          <t>Mental exertion expended on a behaviour that is medium.</t>
         </is>
       </c>
       <c r="D60" s="3" t="n"/>
       <c r="E60" s="3" t="n"/>
-      <c r="F60" s="3" t="n"/>
-      <c r="G60" s="3" t="inlineStr">
-        <is>
-          <t>physical exertion expended on a behaviour</t>
-        </is>
-      </c>
-      <c r="H60" s="3" t="n"/>
-      <c r="I60" s="3" t="inlineStr">
+      <c r="F60" s="3" t="inlineStr">
+        <is>
+          <t>mental exertion expended on a behaviour</t>
+        </is>
+      </c>
+      <c r="G60" s="3" t="n"/>
+      <c r="H60" s="3" t="inlineStr">
         <is>
           <t>behaviour</t>
         </is>
       </c>
+      <c r="I60" s="3" t="n"/>
       <c r="J60" s="3" t="n"/>
       <c r="K60" s="3" t="n"/>
       <c r="L60" s="3" t="n"/>
@@ -4183,7 +4161,7 @@
       <c r="N60" s="3" t="n"/>
       <c r="O60" s="3" t="inlineStr">
         <is>
-          <t>Moderate physical exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what moderate exertion means based on the measurement you use).</t>
+          <t>Moderate mental exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what moderate exertion means based on the measurement you use).</t>
         </is>
       </c>
       <c r="P60" s="3" t="n"/>
@@ -4207,121 +4185,123 @@
       <c r="V60" s="3" t="n"/>
     </row>
     <row r="61">
-      <c r="A61" s="2" t="inlineStr">
-        <is>
-          <t>BCIO:013000</t>
-        </is>
-      </c>
-      <c r="B61" s="2" t="inlineStr">
-        <is>
-          <t>participant engagement with behaviour change intervention</t>
-        </is>
-      </c>
-      <c r="C61" s="2" t="inlineStr">
-        <is>
-          <t>Participant engagement with intervention, where the intervention focuses on changing behaviour.</t>
-        </is>
-      </c>
-      <c r="D61" s="2" t="n"/>
-      <c r="E61" s="2" t="n"/>
-      <c r="F61" s="2" t="n"/>
-      <c r="G61" s="2" t="inlineStr">
-        <is>
-          <t>participant engagement with intervention</t>
-        </is>
-      </c>
-      <c r="H61" s="2" t="inlineStr">
-        <is>
-          <t>process</t>
-        </is>
-      </c>
-      <c r="I61" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
-      <c r="J61" s="2" t="n"/>
-      <c r="K61" s="2" t="n"/>
-      <c r="L61" s="2" t="n"/>
-      <c r="M61" s="2" t="inlineStr">
-        <is>
-          <t>BCI engagement</t>
-        </is>
-      </c>
-      <c r="N61" s="2" t="n"/>
-      <c r="O61" s="2" t="n"/>
-      <c r="P61" s="2" t="inlineStr">
-        <is>
-          <t>Includes mental activities and behaviours.</t>
-        </is>
-      </c>
-      <c r="Q61" s="2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="R61" s="2" t="n"/>
-      <c r="S61" s="2" t="inlineStr">
-        <is>
-          <t>JH; RW; PS</t>
-        </is>
-      </c>
-      <c r="T61" s="2" t="inlineStr">
-        <is>
-          <t>Published</t>
-        </is>
-      </c>
-      <c r="U61" s="2" t="n"/>
-      <c r="V61" s="2" t="n"/>
+      <c r="A61" s="3" t="inlineStr">
+        <is>
+          <t>BCIO:050473</t>
+        </is>
+      </c>
+      <c r="B61" s="3" t="inlineStr">
+        <is>
+          <t>moderate physical exertion expended on behaviour</t>
+        </is>
+      </c>
+      <c r="C61" s="3" t="inlineStr">
+        <is>
+          <t>Physical exertion expended on a behaviour that is medium.</t>
+        </is>
+      </c>
+      <c r="D61" s="3" t="n"/>
+      <c r="E61" s="3" t="n"/>
+      <c r="F61" s="3" t="inlineStr">
+        <is>
+          <t>physical exertion expended on a behaviour</t>
+        </is>
+      </c>
+      <c r="G61" s="3" t="n"/>
+      <c r="H61" s="3" t="inlineStr">
+        <is>
+          <t>behaviour</t>
+        </is>
+      </c>
+      <c r="I61" s="3" t="n"/>
+      <c r="J61" s="3" t="n"/>
+      <c r="K61" s="3" t="n"/>
+      <c r="L61" s="3" t="n"/>
+      <c r="M61" s="3" t="n"/>
+      <c r="N61" s="3" t="n"/>
+      <c r="O61" s="3" t="inlineStr">
+        <is>
+          <t>Moderate physical exertion will mean different things depending on how this concept is operationalised. Therefore, when using this class, you would need to operationalise it for the relevant context (e.g., specify what moderate exertion means based on the measurement you use).</t>
+        </is>
+      </c>
+      <c r="P61" s="3" t="n"/>
+      <c r="Q61" s="3" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R61" s="3" t="n"/>
+      <c r="S61" s="3" t="inlineStr">
+        <is>
+          <t>PS</t>
+        </is>
+      </c>
+      <c r="T61" s="3" t="inlineStr">
+        <is>
+          <t>Obsolete</t>
+        </is>
+      </c>
+      <c r="U61" s="3" t="n"/>
+      <c r="V61" s="3" t="n"/>
     </row>
     <row r="62">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>BCIO:050916</t>
+          <t>BCIO:013000</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
         <is>
+          <t>participant engagement with behaviour change intervention</t>
+        </is>
+      </c>
+      <c r="C62" s="2" t="inlineStr">
+        <is>
+          <t>Participant engagement with intervention, where the intervention focuses on changing behaviour.</t>
+        </is>
+      </c>
+      <c r="D62" s="2" t="n"/>
+      <c r="E62" s="2" t="n"/>
+      <c r="F62" s="2" t="inlineStr">
+        <is>
           <t>participant engagement with intervention</t>
         </is>
       </c>
-      <c r="C62" s="2" t="inlineStr">
-        <is>
-          <t>An individual human activity that is performed by someone in an intervention population, prompted by this intervention and influences the effects of the intervention on its outcome.</t>
-        </is>
-      </c>
-      <c r="D62" s="2" t="inlineStr">
-        <is>
-          <t>The extend to someone interacts with an intervention, including their cognitive, emotional and behavioural response (e.g., attending intervention session) to the intervention itself.</t>
-        </is>
-      </c>
-      <c r="E62" s="2" t="n"/>
-      <c r="F62" s="2" t="n"/>
       <c r="G62" s="2" t="inlineStr">
         <is>
-          <t>individual human activity</t>
-        </is>
-      </c>
-      <c r="H62" s="2" t="n"/>
-      <c r="I62" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+          <t>process</t>
+        </is>
+      </c>
+      <c r="H62" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I62" s="2" t="n"/>
       <c r="J62" s="2" t="n"/>
       <c r="K62" s="2" t="n"/>
       <c r="L62" s="2" t="n"/>
-      <c r="M62" s="2" t="n"/>
+      <c r="M62" s="2" t="inlineStr">
+        <is>
+          <t>BCI engagement</t>
+        </is>
+      </c>
       <c r="N62" s="2" t="n"/>
       <c r="O62" s="2" t="n"/>
-      <c r="P62" s="2" t="n"/>
-      <c r="Q62" s="2" t="n">
-        <v>0</v>
+      <c r="P62" s="2" t="inlineStr">
+        <is>
+          <t>Includes mental activities and behaviours.</t>
+        </is>
+      </c>
+      <c r="Q62" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="R62" s="2" t="n"/>
       <c r="S62" s="2" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>JH; RW; PS</t>
         </is>
       </c>
       <c r="T62" s="2" t="inlineStr">
@@ -4335,53 +4315,51 @@
     <row r="63">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>BCIO:034000</t>
+          <t>BCIO:050916</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
         <is>
-          <t>population behaviour</t>
+          <t>participant engagement with intervention</t>
         </is>
       </c>
       <c r="C63" s="2" t="inlineStr">
         <is>
-          <t>An aggregate of individual human behaviours of members of a population.</t>
-        </is>
-      </c>
-      <c r="D63" s="2" t="n"/>
+          <t>An individual human activity that is performed by someone in an intervention population, prompted by this intervention and influences the effects of the intervention on its outcome.</t>
+        </is>
+      </c>
+      <c r="D63" s="2" t="inlineStr">
+        <is>
+          <t>The extend to someone interacts with an intervention, including their cognitive, emotional and behavioural response (e.g., attending intervention session) to the intervention itself.</t>
+        </is>
+      </c>
       <c r="E63" s="2" t="n"/>
-      <c r="F63" s="2" t="n"/>
-      <c r="G63" s="2" t="inlineStr">
-        <is>
-          <t>process</t>
-        </is>
-      </c>
-      <c r="H63" s="2" t="n"/>
-      <c r="I63" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="F63" s="2" t="inlineStr">
+        <is>
+          <t>individual human activity</t>
+        </is>
+      </c>
+      <c r="G63" s="2" t="n"/>
+      <c r="H63" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I63" s="2" t="n"/>
       <c r="J63" s="2" t="n"/>
       <c r="K63" s="2" t="n"/>
       <c r="L63" s="2" t="n"/>
-      <c r="M63" s="2" t="inlineStr">
-        <is>
-          <t>human behaviour</t>
-        </is>
-      </c>
+      <c r="M63" s="2" t="n"/>
       <c r="N63" s="2" t="n"/>
       <c r="O63" s="2" t="n"/>
       <c r="P63" s="2" t="n"/>
-      <c r="Q63" s="2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="Q63" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="R63" s="2" t="n"/>
       <c r="S63" s="2" t="inlineStr">
         <is>
-          <t>JH</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="T63" s="2" t="inlineStr">
@@ -4395,48 +4373,44 @@
     <row r="64">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>BCIO:043000</t>
+          <t>BCIO:034000</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
         <is>
-          <t>process attribute</t>
+          <t>population behaviour</t>
         </is>
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>A process profile that is an attribute of a process.</t>
-        </is>
-      </c>
-      <c r="D64" s="2" t="inlineStr">
-        <is>
-          <t>An attribute of a process.</t>
-        </is>
-      </c>
+          <t>An aggregate of individual human behaviours of members of a population.</t>
+        </is>
+      </c>
+      <c r="D64" s="2" t="n"/>
       <c r="E64" s="2" t="n"/>
-      <c r="F64" s="2" t="n"/>
-      <c r="G64" s="2" t="inlineStr">
-        <is>
-          <t>process profile</t>
-        </is>
-      </c>
-      <c r="H64" s="2" t="n"/>
-      <c r="I64" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="F64" s="2" t="inlineStr">
+        <is>
+          <t>process</t>
+        </is>
+      </c>
+      <c r="G64" s="2" t="n"/>
+      <c r="H64" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I64" s="2" t="n"/>
       <c r="J64" s="2" t="n"/>
       <c r="K64" s="2" t="n"/>
       <c r="L64" s="2" t="n"/>
-      <c r="M64" s="2" t="n"/>
+      <c r="M64" s="2" t="inlineStr">
+        <is>
+          <t>human behaviour</t>
+        </is>
+      </c>
       <c r="N64" s="2" t="n"/>
       <c r="O64" s="2" t="n"/>
-      <c r="P64" s="2" t="inlineStr">
-        <is>
-          <t>This is intended to provide a user-friendly way of representing the way in which processes are manifest. This is somewhat similar to, but not the same as, the class 'specifically dependent continuant' in Basic Formal Ontology which provides a way of representing features of material entities such as age and size. It is formally equivalent to process profile in Basic Formal Ontology.</t>
-        </is>
-      </c>
+      <c r="P64" s="2" t="n"/>
       <c r="Q64" s="2" t="inlineStr">
         <is>
           <t>0</t>
@@ -4459,40 +4433,48 @@
     <row r="65">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>BCIO:050551</t>
+          <t>BCIO:043000</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
         <is>
-          <t>research study sample</t>
+          <t>process attribute</t>
         </is>
       </c>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>A population whose behaviour is studied in a research study.</t>
-        </is>
-      </c>
-      <c r="D65" s="2" t="n"/>
+          <t>A process profile that is an attribute of a process.</t>
+        </is>
+      </c>
+      <c r="D65" s="2" t="inlineStr">
+        <is>
+          <t>An attribute of a process.</t>
+        </is>
+      </c>
       <c r="E65" s="2" t="n"/>
-      <c r="F65" s="2" t="n"/>
-      <c r="G65" s="2" t="inlineStr">
-        <is>
-          <t>human population</t>
-        </is>
-      </c>
-      <c r="H65" s="2" t="n"/>
-      <c r="I65" s="2" t="inlineStr">
-        <is>
-          <t>Upper level</t>
-        </is>
-      </c>
+      <c r="F65" s="2" t="inlineStr">
+        <is>
+          <t>process profile</t>
+        </is>
+      </c>
+      <c r="G65" s="2" t="n"/>
+      <c r="H65" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I65" s="2" t="n"/>
       <c r="J65" s="2" t="n"/>
       <c r="K65" s="2" t="n"/>
       <c r="L65" s="2" t="n"/>
       <c r="M65" s="2" t="n"/>
       <c r="N65" s="2" t="n"/>
       <c r="O65" s="2" t="n"/>
-      <c r="P65" s="2" t="n"/>
+      <c r="P65" s="2" t="inlineStr">
+        <is>
+          <t>This is intended to provide a user-friendly way of representing the way in which processes are manifest. This is somewhat similar to, but not the same as, the class 'specifically dependent continuant' in Basic Formal Ontology which provides a way of representing features of material entities such as age and size. It is formally equivalent to process profile in Basic Formal Ontology.</t>
+        </is>
+      </c>
       <c r="Q65" s="2" t="inlineStr">
         <is>
           <t>0</t>
@@ -4501,7 +4483,7 @@
       <c r="R65" s="2" t="n"/>
       <c r="S65" s="2" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>JH</t>
         </is>
       </c>
       <c r="T65" s="2" t="inlineStr">
@@ -4511,6 +4493,104 @@
       </c>
       <c r="U65" s="2" t="n"/>
       <c r="V65" s="2" t="n"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="inlineStr">
+        <is>
+          <t>BCIO:050551</t>
+        </is>
+      </c>
+      <c r="B66" s="2" t="inlineStr">
+        <is>
+          <t>research study sample</t>
+        </is>
+      </c>
+      <c r="C66" s="2" t="inlineStr">
+        <is>
+          <t>A population whose behaviour is studied in a research study.</t>
+        </is>
+      </c>
+      <c r="D66" s="2" t="n"/>
+      <c r="E66" s="2" t="n"/>
+      <c r="F66" s="2" t="inlineStr">
+        <is>
+          <t>human population</t>
+        </is>
+      </c>
+      <c r="G66" s="2" t="n"/>
+      <c r="H66" s="2" t="inlineStr">
+        <is>
+          <t>Upper level</t>
+        </is>
+      </c>
+      <c r="I66" s="2" t="n"/>
+      <c r="J66" s="2" t="n"/>
+      <c r="K66" s="2" t="n"/>
+      <c r="L66" s="2" t="n"/>
+      <c r="M66" s="2" t="n"/>
+      <c r="N66" s="2" t="n"/>
+      <c r="O66" s="2" t="n"/>
+      <c r="P66" s="2" t="n"/>
+      <c r="Q66" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R66" s="2" t="n"/>
+      <c r="S66" s="2" t="inlineStr">
+        <is>
+          <t>PS</t>
+        </is>
+      </c>
+      <c r="T66" s="2" t="inlineStr">
+        <is>
+          <t>Published</t>
+        </is>
+      </c>
+      <c r="U66" s="2" t="n"/>
+      <c r="V66" s="2" t="n"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>TEST:0001</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>entity</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr"/>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr"/>
+      <c r="L67" t="inlineStr"/>
+      <c r="M67" t="inlineStr"/>
+      <c r="N67" t="inlineStr"/>
+      <c r="O67" t="inlineStr"/>
+      <c r="P67" t="inlineStr"/>
+      <c r="Q67" t="n">
+        <v>0</v>
+      </c>
+      <c r="R67" t="inlineStr"/>
+      <c r="S67" t="inlineStr"/>
+      <c r="T67" t="inlineStr">
+        <is>
+          <t>External</t>
+        </is>
+      </c>
+      <c r="U67" t="inlineStr"/>
+      <c r="V67" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>